<commit_message>
inclusion of real data
</commit_message>
<xml_diff>
--- a/data/fuels.xlsx
+++ b/data/fuels.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\global_shipping_model\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mscle\Documents\Models\global_shipping_model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Fuel_data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
   <si>
     <t>Hydrogen</t>
   </si>
@@ -175,7 +175,7 @@
     <t>gCO2eq/MJ</t>
   </si>
   <si>
-    <t>#gCO2eq/MJ</t>
+    <t>"</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -552,17 +552,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:J42"/>
+      <selection activeCell="B43" sqref="B43:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
-    <col min="3" max="8" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="9.140625" style="1"/>
     <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1096,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:15">
       <c r="B33" s="1" t="s">
         <v>3</v>
       </c>
@@ -1104,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:15">
       <c r="B34" s="1" t="s">
         <v>2</v>
       </c>
@@ -1112,12 +1113,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:15">
       <c r="B35" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:15">
       <c r="B36" s="1" t="s">
         <v>0</v>
       </c>
@@ -1125,78 +1126,187 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:15">
       <c r="B41" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
-      <c r="B42" t="s">
+    <row r="42" spans="1:15">
+      <c r="A42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43" s="1" t="str">
+        <f>+$A$42&amp;B43&amp;$A$42</f>
+        <v>"HFO"</v>
+      </c>
+      <c r="B43" t="s">
         <v>8</v>
       </c>
-      <c r="C42" t="s">
-        <v>43</v>
-      </c>
-      <c r="D42" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" t="s">
-        <v>1</v>
-      </c>
-      <c r="F42" t="s">
-        <v>14</v>
-      </c>
-      <c r="G42" t="s">
-        <v>44</v>
-      </c>
-      <c r="H42" t="s">
-        <v>45</v>
-      </c>
-      <c r="I42" t="s">
-        <v>46</v>
-      </c>
-      <c r="J42" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B43" s="1">
+      <c r="C43" s="1">
         <f>+SUM(D22:D23)</f>
         <v>86</v>
       </c>
-      <c r="C43" s="1">
+      <c r="E43" s="1">
+        <v>86</v>
+      </c>
+      <c r="G43" s="1">
+        <v>86</v>
+      </c>
+      <c r="H43" s="1">
+        <v>86</v>
+      </c>
+      <c r="I43" s="1">
+        <v>66</v>
+      </c>
+      <c r="J43" s="1">
+        <v>73</v>
+      </c>
+      <c r="K43" s="1">
+        <v>94</v>
+      </c>
+      <c r="L43" s="1">
+        <v>90</v>
+      </c>
+      <c r="M43" s="1">
+        <v>2</v>
+      </c>
+      <c r="N43" s="1">
+        <v>2</v>
+      </c>
+      <c r="O43" s="2">
+        <v>0.147222222222222</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" s="1" t="str">
+        <f t="shared" ref="A44:A51" si="0">+$A$42&amp;B44&amp;$A$42</f>
+        <v>"MDO"</v>
+      </c>
+      <c r="B44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="1">
         <f>+SUM(C22:C23)</f>
         <v>86</v>
       </c>
-      <c r="D43" s="1">
+      <c r="E44" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>"LNG"</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="1">
         <f>+SUM(E22:E23)</f>
         <v>66</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E45" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>"LPG"</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="1">
         <f>+SUM(G22:G23)</f>
         <v>73</v>
       </c>
-      <c r="F43" s="1">
+      <c r="E46" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>"MET"</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="1">
         <f>+SUM(H22:H23)</f>
         <v>94</v>
       </c>
-      <c r="G43" s="1">
+      <c r="E47" s="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>"HYB"</v>
+      </c>
+      <c r="B48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" s="1">
         <f>+SUM(L22:L23)</f>
         <v>90</v>
       </c>
-      <c r="H43" s="1">
+      <c r="E48" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>"HYG"</v>
+      </c>
+      <c r="B49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="1">
         <f>+SUM(M22:M23)</f>
         <v>2</v>
       </c>
-      <c r="I43" s="1">
-        <f>+H43</f>
+      <c r="E49" s="1">
         <v>2</v>
       </c>
-      <c r="J43" s="2">
-        <f>+S5/3.6</f>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>"AMM"</v>
+      </c>
+      <c r="B50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50" s="1">
+        <f>+C49</f>
+        <v>2</v>
+      </c>
+      <c r="E50" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>"ELC"</v>
+      </c>
+      <c r="B51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="2">
+        <f>+SUM(S5)/3.6</f>
+        <v>0.14722222222222223</v>
+      </c>
+      <c r="E51" s="1">
         <v>0.14722222222222223</v>
       </c>
     </row>
@@ -1207,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L3"/>
+  <dimension ref="B2:BO35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1225,6 +1335,2067 @@
         <v>11</v>
       </c>
     </row>
+    <row r="26" spans="2:67">
+      <c r="C26">
+        <v>2011</v>
+      </c>
+      <c r="D26">
+        <f>+C26+1</f>
+        <v>2012</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ref="E26:BO26" si="0">+D26+1</f>
+        <v>2013</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>2014</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>2015</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>2017</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>2018</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>2019</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="0"/>
+        <v>2021</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>2022</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="0"/>
+        <v>2023</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="0"/>
+        <v>2026</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="0"/>
+        <v>2027</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="0"/>
+        <v>2028</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="0"/>
+        <v>2029</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="0"/>
+        <v>2030</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="0"/>
+        <v>2031</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="0"/>
+        <v>2032</v>
+      </c>
+      <c r="Y26">
+        <f t="shared" si="0"/>
+        <v>2033</v>
+      </c>
+      <c r="Z26">
+        <f t="shared" si="0"/>
+        <v>2034</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" si="0"/>
+        <v>2035</v>
+      </c>
+      <c r="AB26">
+        <f t="shared" si="0"/>
+        <v>2036</v>
+      </c>
+      <c r="AC26">
+        <f t="shared" si="0"/>
+        <v>2037</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="0"/>
+        <v>2038</v>
+      </c>
+      <c r="AE26">
+        <f t="shared" si="0"/>
+        <v>2039</v>
+      </c>
+      <c r="AF26">
+        <f t="shared" si="0"/>
+        <v>2040</v>
+      </c>
+      <c r="AG26">
+        <f t="shared" si="0"/>
+        <v>2041</v>
+      </c>
+      <c r="AH26">
+        <f t="shared" si="0"/>
+        <v>2042</v>
+      </c>
+      <c r="AI26">
+        <f t="shared" si="0"/>
+        <v>2043</v>
+      </c>
+      <c r="AJ26">
+        <f t="shared" si="0"/>
+        <v>2044</v>
+      </c>
+      <c r="AK26">
+        <f t="shared" si="0"/>
+        <v>2045</v>
+      </c>
+      <c r="AL26">
+        <f t="shared" si="0"/>
+        <v>2046</v>
+      </c>
+      <c r="AM26">
+        <f t="shared" si="0"/>
+        <v>2047</v>
+      </c>
+      <c r="AN26">
+        <f t="shared" si="0"/>
+        <v>2048</v>
+      </c>
+      <c r="AO26">
+        <f t="shared" si="0"/>
+        <v>2049</v>
+      </c>
+      <c r="AP26">
+        <f t="shared" si="0"/>
+        <v>2050</v>
+      </c>
+      <c r="AQ26">
+        <f t="shared" si="0"/>
+        <v>2051</v>
+      </c>
+      <c r="AR26">
+        <f t="shared" si="0"/>
+        <v>2052</v>
+      </c>
+      <c r="AS26">
+        <f t="shared" si="0"/>
+        <v>2053</v>
+      </c>
+      <c r="AT26">
+        <f t="shared" si="0"/>
+        <v>2054</v>
+      </c>
+      <c r="AU26">
+        <f t="shared" si="0"/>
+        <v>2055</v>
+      </c>
+      <c r="AV26">
+        <f t="shared" si="0"/>
+        <v>2056</v>
+      </c>
+      <c r="AW26">
+        <f t="shared" si="0"/>
+        <v>2057</v>
+      </c>
+      <c r="AX26">
+        <f t="shared" si="0"/>
+        <v>2058</v>
+      </c>
+      <c r="AY26">
+        <f t="shared" si="0"/>
+        <v>2059</v>
+      </c>
+      <c r="AZ26">
+        <f t="shared" si="0"/>
+        <v>2060</v>
+      </c>
+      <c r="BA26">
+        <f t="shared" si="0"/>
+        <v>2061</v>
+      </c>
+      <c r="BB26">
+        <f t="shared" si="0"/>
+        <v>2062</v>
+      </c>
+      <c r="BC26">
+        <f t="shared" si="0"/>
+        <v>2063</v>
+      </c>
+      <c r="BD26">
+        <f t="shared" si="0"/>
+        <v>2064</v>
+      </c>
+      <c r="BE26">
+        <f t="shared" si="0"/>
+        <v>2065</v>
+      </c>
+      <c r="BF26">
+        <f t="shared" si="0"/>
+        <v>2066</v>
+      </c>
+      <c r="BG26">
+        <f t="shared" si="0"/>
+        <v>2067</v>
+      </c>
+      <c r="BH26">
+        <f t="shared" si="0"/>
+        <v>2068</v>
+      </c>
+      <c r="BI26">
+        <f t="shared" si="0"/>
+        <v>2069</v>
+      </c>
+      <c r="BJ26">
+        <f t="shared" si="0"/>
+        <v>2070</v>
+      </c>
+      <c r="BK26">
+        <f t="shared" si="0"/>
+        <v>2071</v>
+      </c>
+      <c r="BL26">
+        <f t="shared" si="0"/>
+        <v>2072</v>
+      </c>
+      <c r="BM26">
+        <f t="shared" si="0"/>
+        <v>2073</v>
+      </c>
+      <c r="BN26">
+        <f t="shared" si="0"/>
+        <v>2074</v>
+      </c>
+      <c r="BO26">
+        <f t="shared" si="0"/>
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="27" spans="2:67">
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>0.75</v>
+      </c>
+      <c r="D27">
+        <v>0.75</v>
+      </c>
+      <c r="E27">
+        <v>0.75</v>
+      </c>
+      <c r="F27">
+        <v>0.75</v>
+      </c>
+      <c r="G27">
+        <v>0.75</v>
+      </c>
+      <c r="H27">
+        <v>0.75</v>
+      </c>
+      <c r="I27">
+        <v>0.75</v>
+      </c>
+      <c r="J27">
+        <v>0.75</v>
+      </c>
+      <c r="K27">
+        <v>0.75</v>
+      </c>
+      <c r="L27">
+        <v>0.75</v>
+      </c>
+      <c r="M27">
+        <v>0.75</v>
+      </c>
+      <c r="N27">
+        <v>0.75</v>
+      </c>
+      <c r="O27">
+        <v>0.75</v>
+      </c>
+      <c r="P27">
+        <v>0.75</v>
+      </c>
+      <c r="Q27">
+        <v>0.75</v>
+      </c>
+      <c r="R27">
+        <v>0.75</v>
+      </c>
+      <c r="S27">
+        <v>0.75</v>
+      </c>
+      <c r="T27">
+        <v>0.75</v>
+      </c>
+      <c r="U27">
+        <v>0.75</v>
+      </c>
+      <c r="V27">
+        <v>0.75</v>
+      </c>
+      <c r="W27">
+        <v>0.75</v>
+      </c>
+      <c r="X27">
+        <v>0.75</v>
+      </c>
+      <c r="Y27">
+        <v>0.75</v>
+      </c>
+      <c r="Z27">
+        <v>0.75</v>
+      </c>
+      <c r="AA27">
+        <v>0.75</v>
+      </c>
+      <c r="AB27">
+        <v>0.75</v>
+      </c>
+      <c r="AC27">
+        <v>0.75</v>
+      </c>
+      <c r="AD27">
+        <v>0.75</v>
+      </c>
+      <c r="AE27">
+        <v>0.75</v>
+      </c>
+      <c r="AF27">
+        <v>0.75</v>
+      </c>
+      <c r="AG27">
+        <v>0.75</v>
+      </c>
+      <c r="AH27">
+        <v>0.75</v>
+      </c>
+      <c r="AI27">
+        <v>0.75</v>
+      </c>
+      <c r="AJ27">
+        <v>0.75</v>
+      </c>
+      <c r="AK27">
+        <v>0.75</v>
+      </c>
+      <c r="AL27">
+        <v>0.75</v>
+      </c>
+      <c r="AM27">
+        <v>0.75</v>
+      </c>
+      <c r="AN27">
+        <v>0.75</v>
+      </c>
+      <c r="AO27">
+        <v>0.75</v>
+      </c>
+      <c r="AP27">
+        <v>0.75</v>
+      </c>
+      <c r="AQ27">
+        <v>0.75</v>
+      </c>
+      <c r="AR27">
+        <v>0.75</v>
+      </c>
+      <c r="AS27">
+        <v>0.75</v>
+      </c>
+      <c r="AT27">
+        <v>0.75</v>
+      </c>
+      <c r="AU27">
+        <v>0.75</v>
+      </c>
+      <c r="AV27">
+        <v>0.75</v>
+      </c>
+      <c r="AW27">
+        <v>0.75</v>
+      </c>
+      <c r="AX27">
+        <v>0.75</v>
+      </c>
+      <c r="AY27">
+        <v>0.75</v>
+      </c>
+      <c r="AZ27">
+        <v>0.75</v>
+      </c>
+      <c r="BA27">
+        <v>0.75</v>
+      </c>
+      <c r="BB27">
+        <v>0.75</v>
+      </c>
+      <c r="BC27">
+        <v>0.75</v>
+      </c>
+      <c r="BD27">
+        <v>0.75</v>
+      </c>
+      <c r="BE27">
+        <v>0.75</v>
+      </c>
+      <c r="BF27">
+        <v>0.75</v>
+      </c>
+      <c r="BG27">
+        <v>0.75</v>
+      </c>
+      <c r="BH27">
+        <v>0.75</v>
+      </c>
+      <c r="BI27">
+        <v>0.75</v>
+      </c>
+      <c r="BJ27">
+        <v>0.75</v>
+      </c>
+      <c r="BK27">
+        <v>0.75</v>
+      </c>
+      <c r="BL27">
+        <v>0.75</v>
+      </c>
+      <c r="BM27">
+        <v>0.75</v>
+      </c>
+      <c r="BN27">
+        <v>0.75</v>
+      </c>
+      <c r="BO27">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="28" spans="2:67">
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28">
+        <v>1.25</v>
+      </c>
+      <c r="D28">
+        <v>1.25</v>
+      </c>
+      <c r="E28">
+        <v>1.25</v>
+      </c>
+      <c r="F28">
+        <v>1.25</v>
+      </c>
+      <c r="G28">
+        <v>1.25</v>
+      </c>
+      <c r="H28">
+        <v>1.25</v>
+      </c>
+      <c r="I28">
+        <v>1.25</v>
+      </c>
+      <c r="J28">
+        <v>1.25</v>
+      </c>
+      <c r="K28">
+        <v>1.25</v>
+      </c>
+      <c r="L28">
+        <v>1.25</v>
+      </c>
+      <c r="M28">
+        <v>1.25</v>
+      </c>
+      <c r="N28">
+        <v>1.25</v>
+      </c>
+      <c r="O28">
+        <v>1.25</v>
+      </c>
+      <c r="P28">
+        <v>1.25</v>
+      </c>
+      <c r="Q28">
+        <v>1.25</v>
+      </c>
+      <c r="R28">
+        <v>1.25</v>
+      </c>
+      <c r="S28">
+        <v>1.25</v>
+      </c>
+      <c r="T28">
+        <v>1.25</v>
+      </c>
+      <c r="U28">
+        <v>1.25</v>
+      </c>
+      <c r="V28">
+        <v>1.25</v>
+      </c>
+      <c r="W28">
+        <v>1.25</v>
+      </c>
+      <c r="X28">
+        <v>1.25</v>
+      </c>
+      <c r="Y28">
+        <v>1.25</v>
+      </c>
+      <c r="Z28">
+        <v>1.25</v>
+      </c>
+      <c r="AA28">
+        <v>1.25</v>
+      </c>
+      <c r="AB28">
+        <v>1.25</v>
+      </c>
+      <c r="AC28">
+        <v>1.25</v>
+      </c>
+      <c r="AD28">
+        <v>1.25</v>
+      </c>
+      <c r="AE28">
+        <v>1.25</v>
+      </c>
+      <c r="AF28">
+        <v>1.25</v>
+      </c>
+      <c r="AG28">
+        <v>1.25</v>
+      </c>
+      <c r="AH28">
+        <v>1.25</v>
+      </c>
+      <c r="AI28">
+        <v>1.25</v>
+      </c>
+      <c r="AJ28">
+        <v>1.25</v>
+      </c>
+      <c r="AK28">
+        <v>1.25</v>
+      </c>
+      <c r="AL28">
+        <v>1.25</v>
+      </c>
+      <c r="AM28">
+        <v>1.25</v>
+      </c>
+      <c r="AN28">
+        <v>1.25</v>
+      </c>
+      <c r="AO28">
+        <v>1.25</v>
+      </c>
+      <c r="AP28">
+        <v>1.25</v>
+      </c>
+      <c r="AQ28">
+        <v>1.25</v>
+      </c>
+      <c r="AR28">
+        <v>1.25</v>
+      </c>
+      <c r="AS28">
+        <v>1.25</v>
+      </c>
+      <c r="AT28">
+        <v>1.25</v>
+      </c>
+      <c r="AU28">
+        <v>1.25</v>
+      </c>
+      <c r="AV28">
+        <v>1.25</v>
+      </c>
+      <c r="AW28">
+        <v>1.25</v>
+      </c>
+      <c r="AX28">
+        <v>1.25</v>
+      </c>
+      <c r="AY28">
+        <v>1.25</v>
+      </c>
+      <c r="AZ28">
+        <v>1.25</v>
+      </c>
+      <c r="BA28">
+        <v>1.25</v>
+      </c>
+      <c r="BB28">
+        <v>1.25</v>
+      </c>
+      <c r="BC28">
+        <v>1.25</v>
+      </c>
+      <c r="BD28">
+        <v>1.25</v>
+      </c>
+      <c r="BE28">
+        <v>1.25</v>
+      </c>
+      <c r="BF28">
+        <v>1.25</v>
+      </c>
+      <c r="BG28">
+        <v>1.25</v>
+      </c>
+      <c r="BH28">
+        <v>1.25</v>
+      </c>
+      <c r="BI28">
+        <v>1.25</v>
+      </c>
+      <c r="BJ28">
+        <v>1.25</v>
+      </c>
+      <c r="BK28">
+        <v>1.25</v>
+      </c>
+      <c r="BL28">
+        <v>1.25</v>
+      </c>
+      <c r="BM28">
+        <v>1.25</v>
+      </c>
+      <c r="BN28">
+        <v>1.25</v>
+      </c>
+      <c r="BO28">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="29" spans="2:67">
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>0.8</v>
+      </c>
+      <c r="D29">
+        <v>0.8</v>
+      </c>
+      <c r="E29">
+        <v>0.8</v>
+      </c>
+      <c r="F29">
+        <v>0.8</v>
+      </c>
+      <c r="G29">
+        <v>0.8</v>
+      </c>
+      <c r="H29">
+        <v>0.8</v>
+      </c>
+      <c r="I29">
+        <v>0.8</v>
+      </c>
+      <c r="J29">
+        <v>0.8</v>
+      </c>
+      <c r="K29">
+        <v>0.8</v>
+      </c>
+      <c r="L29">
+        <v>0.8</v>
+      </c>
+      <c r="M29">
+        <v>0.8</v>
+      </c>
+      <c r="N29">
+        <v>0.8</v>
+      </c>
+      <c r="O29">
+        <v>0.8</v>
+      </c>
+      <c r="P29">
+        <v>0.8</v>
+      </c>
+      <c r="Q29">
+        <v>0.8</v>
+      </c>
+      <c r="R29">
+        <v>0.8</v>
+      </c>
+      <c r="S29">
+        <v>0.8</v>
+      </c>
+      <c r="T29">
+        <v>0.8</v>
+      </c>
+      <c r="U29">
+        <v>0.8</v>
+      </c>
+      <c r="V29">
+        <v>0.8</v>
+      </c>
+      <c r="W29">
+        <v>0.8</v>
+      </c>
+      <c r="X29">
+        <v>0.8</v>
+      </c>
+      <c r="Y29">
+        <v>0.8</v>
+      </c>
+      <c r="Z29">
+        <v>0.8</v>
+      </c>
+      <c r="AA29">
+        <v>0.8</v>
+      </c>
+      <c r="AB29">
+        <v>0.8</v>
+      </c>
+      <c r="AC29">
+        <v>0.8</v>
+      </c>
+      <c r="AD29">
+        <v>0.8</v>
+      </c>
+      <c r="AE29">
+        <v>0.8</v>
+      </c>
+      <c r="AF29">
+        <v>0.8</v>
+      </c>
+      <c r="AG29">
+        <v>0.8</v>
+      </c>
+      <c r="AH29">
+        <v>0.8</v>
+      </c>
+      <c r="AI29">
+        <v>0.8</v>
+      </c>
+      <c r="AJ29">
+        <v>0.8</v>
+      </c>
+      <c r="AK29">
+        <v>0.8</v>
+      </c>
+      <c r="AL29">
+        <v>0.8</v>
+      </c>
+      <c r="AM29">
+        <v>0.8</v>
+      </c>
+      <c r="AN29">
+        <v>0.8</v>
+      </c>
+      <c r="AO29">
+        <v>0.8</v>
+      </c>
+      <c r="AP29">
+        <v>0.8</v>
+      </c>
+      <c r="AQ29">
+        <v>0.8</v>
+      </c>
+      <c r="AR29">
+        <v>0.8</v>
+      </c>
+      <c r="AS29">
+        <v>0.8</v>
+      </c>
+      <c r="AT29">
+        <v>0.8</v>
+      </c>
+      <c r="AU29">
+        <v>0.8</v>
+      </c>
+      <c r="AV29">
+        <v>0.8</v>
+      </c>
+      <c r="AW29">
+        <v>0.8</v>
+      </c>
+      <c r="AX29">
+        <v>0.8</v>
+      </c>
+      <c r="AY29">
+        <v>0.8</v>
+      </c>
+      <c r="AZ29">
+        <v>0.8</v>
+      </c>
+      <c r="BA29">
+        <v>0.8</v>
+      </c>
+      <c r="BB29">
+        <v>0.8</v>
+      </c>
+      <c r="BC29">
+        <v>0.8</v>
+      </c>
+      <c r="BD29">
+        <v>0.8</v>
+      </c>
+      <c r="BE29">
+        <v>0.8</v>
+      </c>
+      <c r="BF29">
+        <v>0.8</v>
+      </c>
+      <c r="BG29">
+        <v>0.8</v>
+      </c>
+      <c r="BH29">
+        <v>0.8</v>
+      </c>
+      <c r="BI29">
+        <v>0.8</v>
+      </c>
+      <c r="BJ29">
+        <v>0.8</v>
+      </c>
+      <c r="BK29">
+        <v>0.8</v>
+      </c>
+      <c r="BL29">
+        <v>0.8</v>
+      </c>
+      <c r="BM29">
+        <v>0.8</v>
+      </c>
+      <c r="BN29">
+        <v>0.8</v>
+      </c>
+      <c r="BO29">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:67">
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0.9</v>
+      </c>
+      <c r="D30">
+        <v>0.9</v>
+      </c>
+      <c r="E30">
+        <v>0.9</v>
+      </c>
+      <c r="F30">
+        <v>0.9</v>
+      </c>
+      <c r="G30">
+        <v>0.9</v>
+      </c>
+      <c r="H30">
+        <v>0.9</v>
+      </c>
+      <c r="I30">
+        <v>0.9</v>
+      </c>
+      <c r="J30">
+        <v>0.9</v>
+      </c>
+      <c r="K30">
+        <v>0.9</v>
+      </c>
+      <c r="L30">
+        <v>0.9</v>
+      </c>
+      <c r="M30">
+        <v>0.9</v>
+      </c>
+      <c r="N30">
+        <v>0.9</v>
+      </c>
+      <c r="O30">
+        <v>0.9</v>
+      </c>
+      <c r="P30">
+        <v>0.9</v>
+      </c>
+      <c r="Q30">
+        <v>0.9</v>
+      </c>
+      <c r="R30">
+        <v>0.9</v>
+      </c>
+      <c r="S30">
+        <v>0.9</v>
+      </c>
+      <c r="T30">
+        <v>0.9</v>
+      </c>
+      <c r="U30">
+        <v>0.9</v>
+      </c>
+      <c r="V30">
+        <v>0.9</v>
+      </c>
+      <c r="W30">
+        <v>0.9</v>
+      </c>
+      <c r="X30">
+        <v>0.9</v>
+      </c>
+      <c r="Y30">
+        <v>0.9</v>
+      </c>
+      <c r="Z30">
+        <v>0.9</v>
+      </c>
+      <c r="AA30">
+        <v>0.9</v>
+      </c>
+      <c r="AB30">
+        <v>0.9</v>
+      </c>
+      <c r="AC30">
+        <v>0.9</v>
+      </c>
+      <c r="AD30">
+        <v>0.9</v>
+      </c>
+      <c r="AE30">
+        <v>0.9</v>
+      </c>
+      <c r="AF30">
+        <v>0.9</v>
+      </c>
+      <c r="AG30">
+        <v>0.9</v>
+      </c>
+      <c r="AH30">
+        <v>0.9</v>
+      </c>
+      <c r="AI30">
+        <v>0.9</v>
+      </c>
+      <c r="AJ30">
+        <v>0.9</v>
+      </c>
+      <c r="AK30">
+        <v>0.9</v>
+      </c>
+      <c r="AL30">
+        <v>0.9</v>
+      </c>
+      <c r="AM30">
+        <v>0.9</v>
+      </c>
+      <c r="AN30">
+        <v>0.9</v>
+      </c>
+      <c r="AO30">
+        <v>0.9</v>
+      </c>
+      <c r="AP30">
+        <v>0.9</v>
+      </c>
+      <c r="AQ30">
+        <v>0.9</v>
+      </c>
+      <c r="AR30">
+        <v>0.9</v>
+      </c>
+      <c r="AS30">
+        <v>0.9</v>
+      </c>
+      <c r="AT30">
+        <v>0.9</v>
+      </c>
+      <c r="AU30">
+        <v>0.9</v>
+      </c>
+      <c r="AV30">
+        <v>0.9</v>
+      </c>
+      <c r="AW30">
+        <v>0.9</v>
+      </c>
+      <c r="AX30">
+        <v>0.9</v>
+      </c>
+      <c r="AY30">
+        <v>0.9</v>
+      </c>
+      <c r="AZ30">
+        <v>0.9</v>
+      </c>
+      <c r="BA30">
+        <v>0.9</v>
+      </c>
+      <c r="BB30">
+        <v>0.9</v>
+      </c>
+      <c r="BC30">
+        <v>0.9</v>
+      </c>
+      <c r="BD30">
+        <v>0.9</v>
+      </c>
+      <c r="BE30">
+        <v>0.9</v>
+      </c>
+      <c r="BF30">
+        <v>0.9</v>
+      </c>
+      <c r="BG30">
+        <v>0.9</v>
+      </c>
+      <c r="BH30">
+        <v>0.9</v>
+      </c>
+      <c r="BI30">
+        <v>0.9</v>
+      </c>
+      <c r="BJ30">
+        <v>0.9</v>
+      </c>
+      <c r="BK30">
+        <v>0.9</v>
+      </c>
+      <c r="BL30">
+        <v>0.9</v>
+      </c>
+      <c r="BM30">
+        <v>0.9</v>
+      </c>
+      <c r="BN30">
+        <v>0.9</v>
+      </c>
+      <c r="BO30">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:67">
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>1.2</v>
+      </c>
+      <c r="D31">
+        <v>1.2</v>
+      </c>
+      <c r="E31">
+        <v>1.2</v>
+      </c>
+      <c r="F31">
+        <v>1.2</v>
+      </c>
+      <c r="G31">
+        <v>1.2</v>
+      </c>
+      <c r="H31">
+        <v>1.2</v>
+      </c>
+      <c r="I31">
+        <v>1.2</v>
+      </c>
+      <c r="J31">
+        <v>1.2</v>
+      </c>
+      <c r="K31">
+        <v>1.2</v>
+      </c>
+      <c r="L31">
+        <v>1.2</v>
+      </c>
+      <c r="M31">
+        <v>1.2</v>
+      </c>
+      <c r="N31">
+        <v>1.2</v>
+      </c>
+      <c r="O31">
+        <v>1.2</v>
+      </c>
+      <c r="P31">
+        <v>1.2</v>
+      </c>
+      <c r="Q31">
+        <v>1.2</v>
+      </c>
+      <c r="R31">
+        <v>1.2</v>
+      </c>
+      <c r="S31">
+        <v>1.2</v>
+      </c>
+      <c r="T31">
+        <v>1.2</v>
+      </c>
+      <c r="U31">
+        <v>1.2</v>
+      </c>
+      <c r="V31">
+        <v>1.2</v>
+      </c>
+      <c r="W31">
+        <v>1.2</v>
+      </c>
+      <c r="X31">
+        <v>1.2</v>
+      </c>
+      <c r="Y31">
+        <v>1.2</v>
+      </c>
+      <c r="Z31">
+        <v>1.2</v>
+      </c>
+      <c r="AA31">
+        <v>1.2</v>
+      </c>
+      <c r="AB31">
+        <v>1.2</v>
+      </c>
+      <c r="AC31">
+        <v>1.2</v>
+      </c>
+      <c r="AD31">
+        <v>1.2</v>
+      </c>
+      <c r="AE31">
+        <v>1.2</v>
+      </c>
+      <c r="AF31">
+        <v>1.2</v>
+      </c>
+      <c r="AG31">
+        <v>1.2</v>
+      </c>
+      <c r="AH31">
+        <v>1.2</v>
+      </c>
+      <c r="AI31">
+        <v>1.2</v>
+      </c>
+      <c r="AJ31">
+        <v>1.2</v>
+      </c>
+      <c r="AK31">
+        <v>1.2</v>
+      </c>
+      <c r="AL31">
+        <v>1.2</v>
+      </c>
+      <c r="AM31">
+        <v>1.2</v>
+      </c>
+      <c r="AN31">
+        <v>1.2</v>
+      </c>
+      <c r="AO31">
+        <v>1.2</v>
+      </c>
+      <c r="AP31">
+        <v>1.2</v>
+      </c>
+      <c r="AQ31">
+        <v>1.2</v>
+      </c>
+      <c r="AR31">
+        <v>1.2</v>
+      </c>
+      <c r="AS31">
+        <v>1.2</v>
+      </c>
+      <c r="AT31">
+        <v>1.2</v>
+      </c>
+      <c r="AU31">
+        <v>1.2</v>
+      </c>
+      <c r="AV31">
+        <v>1.2</v>
+      </c>
+      <c r="AW31">
+        <v>1.2</v>
+      </c>
+      <c r="AX31">
+        <v>1.2</v>
+      </c>
+      <c r="AY31">
+        <v>1.2</v>
+      </c>
+      <c r="AZ31">
+        <v>1.2</v>
+      </c>
+      <c r="BA31">
+        <v>1.2</v>
+      </c>
+      <c r="BB31">
+        <v>1.2</v>
+      </c>
+      <c r="BC31">
+        <v>1.2</v>
+      </c>
+      <c r="BD31">
+        <v>1.2</v>
+      </c>
+      <c r="BE31">
+        <v>1.2</v>
+      </c>
+      <c r="BF31">
+        <v>1.2</v>
+      </c>
+      <c r="BG31">
+        <v>1.2</v>
+      </c>
+      <c r="BH31">
+        <v>1.2</v>
+      </c>
+      <c r="BI31">
+        <v>1.2</v>
+      </c>
+      <c r="BJ31">
+        <v>1.2</v>
+      </c>
+      <c r="BK31">
+        <v>1.2</v>
+      </c>
+      <c r="BL31">
+        <v>1.2</v>
+      </c>
+      <c r="BM31">
+        <v>1.2</v>
+      </c>
+      <c r="BN31">
+        <v>1.2</v>
+      </c>
+      <c r="BO31">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:67">
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32">
+        <v>1.3</v>
+      </c>
+      <c r="D32">
+        <v>1.3</v>
+      </c>
+      <c r="E32">
+        <v>1.3</v>
+      </c>
+      <c r="F32">
+        <v>1.3</v>
+      </c>
+      <c r="G32">
+        <v>1.3</v>
+      </c>
+      <c r="H32">
+        <v>1.3</v>
+      </c>
+      <c r="I32">
+        <v>1.3</v>
+      </c>
+      <c r="J32">
+        <v>1.3</v>
+      </c>
+      <c r="K32">
+        <v>1.3</v>
+      </c>
+      <c r="L32">
+        <v>1.3</v>
+      </c>
+      <c r="M32">
+        <v>1.3</v>
+      </c>
+      <c r="N32">
+        <v>1.3</v>
+      </c>
+      <c r="O32">
+        <v>1.3</v>
+      </c>
+      <c r="P32">
+        <v>1.3</v>
+      </c>
+      <c r="Q32">
+        <v>1.3</v>
+      </c>
+      <c r="R32">
+        <v>1.3</v>
+      </c>
+      <c r="S32">
+        <v>1.3</v>
+      </c>
+      <c r="T32">
+        <v>1.3</v>
+      </c>
+      <c r="U32">
+        <v>1.3</v>
+      </c>
+      <c r="V32">
+        <v>1.3</v>
+      </c>
+      <c r="W32">
+        <v>1.3</v>
+      </c>
+      <c r="X32">
+        <v>1.3</v>
+      </c>
+      <c r="Y32">
+        <v>1.3</v>
+      </c>
+      <c r="Z32">
+        <v>1.3</v>
+      </c>
+      <c r="AA32">
+        <v>1.3</v>
+      </c>
+      <c r="AB32">
+        <v>1.3</v>
+      </c>
+      <c r="AC32">
+        <v>1.3</v>
+      </c>
+      <c r="AD32">
+        <v>1.3</v>
+      </c>
+      <c r="AE32">
+        <v>1.3</v>
+      </c>
+      <c r="AF32">
+        <v>1.3</v>
+      </c>
+      <c r="AG32">
+        <v>1.3</v>
+      </c>
+      <c r="AH32">
+        <v>1.3</v>
+      </c>
+      <c r="AI32">
+        <v>1.3</v>
+      </c>
+      <c r="AJ32">
+        <v>1.3</v>
+      </c>
+      <c r="AK32">
+        <v>1.3</v>
+      </c>
+      <c r="AL32">
+        <v>1.3</v>
+      </c>
+      <c r="AM32">
+        <v>1.3</v>
+      </c>
+      <c r="AN32">
+        <v>1.3</v>
+      </c>
+      <c r="AO32">
+        <v>1.3</v>
+      </c>
+      <c r="AP32">
+        <v>1.3</v>
+      </c>
+      <c r="AQ32">
+        <v>1.3</v>
+      </c>
+      <c r="AR32">
+        <v>1.3</v>
+      </c>
+      <c r="AS32">
+        <v>1.3</v>
+      </c>
+      <c r="AT32">
+        <v>1.3</v>
+      </c>
+      <c r="AU32">
+        <v>1.3</v>
+      </c>
+      <c r="AV32">
+        <v>1.3</v>
+      </c>
+      <c r="AW32">
+        <v>1.3</v>
+      </c>
+      <c r="AX32">
+        <v>1.3</v>
+      </c>
+      <c r="AY32">
+        <v>1.3</v>
+      </c>
+      <c r="AZ32">
+        <v>1.3</v>
+      </c>
+      <c r="BA32">
+        <v>1.3</v>
+      </c>
+      <c r="BB32">
+        <v>1.3</v>
+      </c>
+      <c r="BC32">
+        <v>1.3</v>
+      </c>
+      <c r="BD32">
+        <v>1.3</v>
+      </c>
+      <c r="BE32">
+        <v>1.3</v>
+      </c>
+      <c r="BF32">
+        <v>1.3</v>
+      </c>
+      <c r="BG32">
+        <v>1.3</v>
+      </c>
+      <c r="BH32">
+        <v>1.3</v>
+      </c>
+      <c r="BI32">
+        <v>1.3</v>
+      </c>
+      <c r="BJ32">
+        <v>1.3</v>
+      </c>
+      <c r="BK32">
+        <v>1.3</v>
+      </c>
+      <c r="BL32">
+        <v>1.3</v>
+      </c>
+      <c r="BM32">
+        <v>1.3</v>
+      </c>
+      <c r="BN32">
+        <v>1.3</v>
+      </c>
+      <c r="BO32">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:67">
+      <c r="B33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33">
+        <v>1.3</v>
+      </c>
+      <c r="D33">
+        <v>1.3</v>
+      </c>
+      <c r="E33">
+        <v>1.3</v>
+      </c>
+      <c r="F33">
+        <v>1.3</v>
+      </c>
+      <c r="G33">
+        <v>1.3</v>
+      </c>
+      <c r="H33">
+        <v>1.3</v>
+      </c>
+      <c r="I33">
+        <v>1.3</v>
+      </c>
+      <c r="J33">
+        <v>1.3</v>
+      </c>
+      <c r="K33">
+        <v>1.3</v>
+      </c>
+      <c r="L33">
+        <v>1.3</v>
+      </c>
+      <c r="M33">
+        <v>1.3</v>
+      </c>
+      <c r="N33">
+        <v>1.3</v>
+      </c>
+      <c r="O33">
+        <v>1.3</v>
+      </c>
+      <c r="P33">
+        <v>1.3</v>
+      </c>
+      <c r="Q33">
+        <v>1.3</v>
+      </c>
+      <c r="R33">
+        <v>1.3</v>
+      </c>
+      <c r="S33">
+        <v>1.3</v>
+      </c>
+      <c r="T33">
+        <v>1.3</v>
+      </c>
+      <c r="U33">
+        <v>1.3</v>
+      </c>
+      <c r="V33">
+        <v>1.3</v>
+      </c>
+      <c r="W33">
+        <v>1.3</v>
+      </c>
+      <c r="X33">
+        <v>1.3</v>
+      </c>
+      <c r="Y33">
+        <v>1.3</v>
+      </c>
+      <c r="Z33">
+        <v>1.3</v>
+      </c>
+      <c r="AA33">
+        <v>1.3</v>
+      </c>
+      <c r="AB33">
+        <v>1.3</v>
+      </c>
+      <c r="AC33">
+        <v>1.3</v>
+      </c>
+      <c r="AD33">
+        <v>1.3</v>
+      </c>
+      <c r="AE33">
+        <v>1.3</v>
+      </c>
+      <c r="AF33">
+        <v>1.3</v>
+      </c>
+      <c r="AG33">
+        <v>1.3</v>
+      </c>
+      <c r="AH33">
+        <v>1.3</v>
+      </c>
+      <c r="AI33">
+        <v>1.3</v>
+      </c>
+      <c r="AJ33">
+        <v>1.3</v>
+      </c>
+      <c r="AK33">
+        <v>1.3</v>
+      </c>
+      <c r="AL33">
+        <v>1.3</v>
+      </c>
+      <c r="AM33">
+        <v>1.3</v>
+      </c>
+      <c r="AN33">
+        <v>1.3</v>
+      </c>
+      <c r="AO33">
+        <v>1.3</v>
+      </c>
+      <c r="AP33">
+        <v>1.3</v>
+      </c>
+      <c r="AQ33">
+        <v>1.3</v>
+      </c>
+      <c r="AR33">
+        <v>1.3</v>
+      </c>
+      <c r="AS33">
+        <v>1.3</v>
+      </c>
+      <c r="AT33">
+        <v>1.3</v>
+      </c>
+      <c r="AU33">
+        <v>1.3</v>
+      </c>
+      <c r="AV33">
+        <v>1.3</v>
+      </c>
+      <c r="AW33">
+        <v>1.3</v>
+      </c>
+      <c r="AX33">
+        <v>1.3</v>
+      </c>
+      <c r="AY33">
+        <v>1.3</v>
+      </c>
+      <c r="AZ33">
+        <v>1.3</v>
+      </c>
+      <c r="BA33">
+        <v>1.3</v>
+      </c>
+      <c r="BB33">
+        <v>1.3</v>
+      </c>
+      <c r="BC33">
+        <v>1.3</v>
+      </c>
+      <c r="BD33">
+        <v>1.3</v>
+      </c>
+      <c r="BE33">
+        <v>1.3</v>
+      </c>
+      <c r="BF33">
+        <v>1.3</v>
+      </c>
+      <c r="BG33">
+        <v>1.3</v>
+      </c>
+      <c r="BH33">
+        <v>1.3</v>
+      </c>
+      <c r="BI33">
+        <v>1.3</v>
+      </c>
+      <c r="BJ33">
+        <v>1.3</v>
+      </c>
+      <c r="BK33">
+        <v>1.3</v>
+      </c>
+      <c r="BL33">
+        <v>1.3</v>
+      </c>
+      <c r="BM33">
+        <v>1.3</v>
+      </c>
+      <c r="BN33">
+        <v>1.3</v>
+      </c>
+      <c r="BO33">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:67">
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34">
+        <v>1.3</v>
+      </c>
+      <c r="D34">
+        <v>1.3</v>
+      </c>
+      <c r="E34">
+        <v>1.3</v>
+      </c>
+      <c r="F34">
+        <v>1.3</v>
+      </c>
+      <c r="G34">
+        <v>1.3</v>
+      </c>
+      <c r="H34">
+        <v>1.3</v>
+      </c>
+      <c r="I34">
+        <v>1.3</v>
+      </c>
+      <c r="J34">
+        <v>1.3</v>
+      </c>
+      <c r="K34">
+        <v>1.3</v>
+      </c>
+      <c r="L34">
+        <v>1.3</v>
+      </c>
+      <c r="M34">
+        <v>1.3</v>
+      </c>
+      <c r="N34">
+        <v>1.3</v>
+      </c>
+      <c r="O34">
+        <v>1.3</v>
+      </c>
+      <c r="P34">
+        <v>1.3</v>
+      </c>
+      <c r="Q34">
+        <v>1.3</v>
+      </c>
+      <c r="R34">
+        <v>1.3</v>
+      </c>
+      <c r="S34">
+        <v>1.3</v>
+      </c>
+      <c r="T34">
+        <v>1.3</v>
+      </c>
+      <c r="U34">
+        <v>1.3</v>
+      </c>
+      <c r="V34">
+        <v>1.3</v>
+      </c>
+      <c r="W34">
+        <v>1.3</v>
+      </c>
+      <c r="X34">
+        <v>1.3</v>
+      </c>
+      <c r="Y34">
+        <v>1.3</v>
+      </c>
+      <c r="Z34">
+        <v>1.3</v>
+      </c>
+      <c r="AA34">
+        <v>1.3</v>
+      </c>
+      <c r="AB34">
+        <v>1.3</v>
+      </c>
+      <c r="AC34">
+        <v>1.3</v>
+      </c>
+      <c r="AD34">
+        <v>1.3</v>
+      </c>
+      <c r="AE34">
+        <v>1.3</v>
+      </c>
+      <c r="AF34">
+        <v>1.3</v>
+      </c>
+      <c r="AG34">
+        <v>1.3</v>
+      </c>
+      <c r="AH34">
+        <v>1.3</v>
+      </c>
+      <c r="AI34">
+        <v>1.3</v>
+      </c>
+      <c r="AJ34">
+        <v>1.3</v>
+      </c>
+      <c r="AK34">
+        <v>1.3</v>
+      </c>
+      <c r="AL34">
+        <v>1.3</v>
+      </c>
+      <c r="AM34">
+        <v>1.3</v>
+      </c>
+      <c r="AN34">
+        <v>1.3</v>
+      </c>
+      <c r="AO34">
+        <v>1.3</v>
+      </c>
+      <c r="AP34">
+        <v>1.3</v>
+      </c>
+      <c r="AQ34">
+        <v>1.3</v>
+      </c>
+      <c r="AR34">
+        <v>1.3</v>
+      </c>
+      <c r="AS34">
+        <v>1.3</v>
+      </c>
+      <c r="AT34">
+        <v>1.3</v>
+      </c>
+      <c r="AU34">
+        <v>1.3</v>
+      </c>
+      <c r="AV34">
+        <v>1.3</v>
+      </c>
+      <c r="AW34">
+        <v>1.3</v>
+      </c>
+      <c r="AX34">
+        <v>1.3</v>
+      </c>
+      <c r="AY34">
+        <v>1.3</v>
+      </c>
+      <c r="AZ34">
+        <v>1.3</v>
+      </c>
+      <c r="BA34">
+        <v>1.3</v>
+      </c>
+      <c r="BB34">
+        <v>1.3</v>
+      </c>
+      <c r="BC34">
+        <v>1.3</v>
+      </c>
+      <c r="BD34">
+        <v>1.3</v>
+      </c>
+      <c r="BE34">
+        <v>1.3</v>
+      </c>
+      <c r="BF34">
+        <v>1.3</v>
+      </c>
+      <c r="BG34">
+        <v>1.3</v>
+      </c>
+      <c r="BH34">
+        <v>1.3</v>
+      </c>
+      <c r="BI34">
+        <v>1.3</v>
+      </c>
+      <c r="BJ34">
+        <v>1.3</v>
+      </c>
+      <c r="BK34">
+        <v>1.3</v>
+      </c>
+      <c r="BL34">
+        <v>1.3</v>
+      </c>
+      <c r="BM34">
+        <v>1.3</v>
+      </c>
+      <c r="BN34">
+        <v>1.3</v>
+      </c>
+      <c r="BO34">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:67">
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35">
+        <v>1.3</v>
+      </c>
+      <c r="D35">
+        <v>1.3</v>
+      </c>
+      <c r="E35">
+        <v>1.3</v>
+      </c>
+      <c r="F35">
+        <v>1.3</v>
+      </c>
+      <c r="G35">
+        <v>1.3</v>
+      </c>
+      <c r="H35">
+        <v>1.3</v>
+      </c>
+      <c r="I35">
+        <v>1.3</v>
+      </c>
+      <c r="J35">
+        <v>1.3</v>
+      </c>
+      <c r="K35">
+        <v>1.3</v>
+      </c>
+      <c r="L35">
+        <v>1.3</v>
+      </c>
+      <c r="M35">
+        <v>1.3</v>
+      </c>
+      <c r="N35">
+        <v>1.3</v>
+      </c>
+      <c r="O35">
+        <v>1.3</v>
+      </c>
+      <c r="P35">
+        <v>1.3</v>
+      </c>
+      <c r="Q35">
+        <v>1.3</v>
+      </c>
+      <c r="R35">
+        <v>1.3</v>
+      </c>
+      <c r="S35">
+        <v>1.3</v>
+      </c>
+      <c r="T35">
+        <v>1.3</v>
+      </c>
+      <c r="U35">
+        <v>1.3</v>
+      </c>
+      <c r="V35">
+        <v>1.3</v>
+      </c>
+      <c r="W35">
+        <v>1.3</v>
+      </c>
+      <c r="X35">
+        <v>1.3</v>
+      </c>
+      <c r="Y35">
+        <v>1.3</v>
+      </c>
+      <c r="Z35">
+        <v>1.3</v>
+      </c>
+      <c r="AA35">
+        <v>1.3</v>
+      </c>
+      <c r="AB35">
+        <v>1.3</v>
+      </c>
+      <c r="AC35">
+        <v>1.3</v>
+      </c>
+      <c r="AD35">
+        <v>1.3</v>
+      </c>
+      <c r="AE35">
+        <v>1.3</v>
+      </c>
+      <c r="AF35">
+        <v>1.3</v>
+      </c>
+      <c r="AG35">
+        <v>1.3</v>
+      </c>
+      <c r="AH35">
+        <v>1.3</v>
+      </c>
+      <c r="AI35">
+        <v>1.3</v>
+      </c>
+      <c r="AJ35">
+        <v>1.3</v>
+      </c>
+      <c r="AK35">
+        <v>1.3</v>
+      </c>
+      <c r="AL35">
+        <v>1.3</v>
+      </c>
+      <c r="AM35">
+        <v>1.3</v>
+      </c>
+      <c r="AN35">
+        <v>1.3</v>
+      </c>
+      <c r="AO35">
+        <v>1.3</v>
+      </c>
+      <c r="AP35">
+        <v>1.3</v>
+      </c>
+      <c r="AQ35">
+        <v>1.3</v>
+      </c>
+      <c r="AR35">
+        <v>1.3</v>
+      </c>
+      <c r="AS35">
+        <v>1.3</v>
+      </c>
+      <c r="AT35">
+        <v>1.3</v>
+      </c>
+      <c r="AU35">
+        <v>1.3</v>
+      </c>
+      <c r="AV35">
+        <v>1.3</v>
+      </c>
+      <c r="AW35">
+        <v>1.3</v>
+      </c>
+      <c r="AX35">
+        <v>1.3</v>
+      </c>
+      <c r="AY35">
+        <v>1.3</v>
+      </c>
+      <c r="AZ35">
+        <v>1.3</v>
+      </c>
+      <c r="BA35">
+        <v>1.3</v>
+      </c>
+      <c r="BB35">
+        <v>1.3</v>
+      </c>
+      <c r="BC35">
+        <v>1.3</v>
+      </c>
+      <c r="BD35">
+        <v>1.3</v>
+      </c>
+      <c r="BE35">
+        <v>1.3</v>
+      </c>
+      <c r="BF35">
+        <v>1.3</v>
+      </c>
+      <c r="BG35">
+        <v>1.3</v>
+      </c>
+      <c r="BH35">
+        <v>1.3</v>
+      </c>
+      <c r="BI35">
+        <v>1.3</v>
+      </c>
+      <c r="BJ35">
+        <v>1.3</v>
+      </c>
+      <c r="BK35">
+        <v>1.3</v>
+      </c>
+      <c r="BL35">
+        <v>1.3</v>
+      </c>
+      <c r="BM35">
+        <v>1.3</v>
+      </c>
+      <c r="BN35">
+        <v>1.3</v>
+      </c>
+      <c r="BO35">
+        <v>1.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
fixed stock constraint, changed emissions to just tank to prop, made output easier to read
</commit_message>
<xml_diff>
--- a/data/fuels.xlsx
+++ b/data/fuels.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fuel_data" sheetId="1" r:id="rId1"/>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43:B51"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="O43" sqref="G43:O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1154,33 +1154,7 @@
       <c r="E43" s="1">
         <v>86</v>
       </c>
-      <c r="G43" s="1">
-        <v>86</v>
-      </c>
-      <c r="H43" s="1">
-        <v>86</v>
-      </c>
-      <c r="I43" s="1">
-        <v>66</v>
-      </c>
-      <c r="J43" s="1">
-        <v>73</v>
-      </c>
-      <c r="K43" s="1">
-        <v>94</v>
-      </c>
-      <c r="L43" s="1">
-        <v>90</v>
-      </c>
-      <c r="M43" s="1">
-        <v>2</v>
-      </c>
-      <c r="N43" s="1">
-        <v>2</v>
-      </c>
-      <c r="O43" s="2">
-        <v>0.147222222222222</v>
-      </c>
+      <c r="O43" s="2"/>
     </row>
     <row r="44" spans="1:15">
       <c r="A44" s="1" t="str">
@@ -1319,7 +1293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BO35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
data updates on transport work  and costs
</commit_message>
<xml_diff>
--- a/data/fuels.xlsx
+++ b/data/fuels.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Fuel_data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
   <si>
     <t>Hydrogen</t>
   </si>
@@ -176,6 +176,21 @@
   </si>
   <si>
     <t>"</t>
+  </si>
+  <si>
+    <t>Lower heating value</t>
+  </si>
+  <si>
+    <t>Ethanol</t>
+  </si>
+  <si>
+    <t>MJ/kg</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study on the use of ethyl and methyl alcohol as alternative fuels in shipping </t>
   </si>
 </sst>
 </file>
@@ -233,16 +248,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>48160</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>86260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>284033</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>37268</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>27362</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -259,8 +274,46 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7686675" y="619660"/>
-          <a:ext cx="7837358" cy="3799108"/>
+          <a:off x="6619875" y="467260"/>
+          <a:ext cx="4989887" cy="2418815"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>8852</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>56911</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12306300" y="619125"/>
+          <a:ext cx="5380952" cy="1914286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -535,17 +588,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B4:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="K6" sqref="K5:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="4" spans="2:11">
+      <c r="C4" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="1">
+        <v>40</v>
+      </c>
+      <c r="F6" s="1">
+        <v>42.7</v>
+      </c>
+      <c r="G6" s="1">
+        <v>50.113999999999997</v>
+      </c>
+      <c r="H6" s="1">
+        <v>19.5</v>
+      </c>
+      <c r="I6" s="1">
+        <v>26.9</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="E7" s="1">
+        <v>40.4</v>
+      </c>
+      <c r="G7" s="1">
+        <v>48.5</v>
+      </c>
+      <c r="H7" s="1">
+        <v>20</v>
+      </c>
+      <c r="I7" s="1">
+        <v>28</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -554,7 +673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="O43" sqref="G43:O43"/>
     </sheetView>
   </sheetViews>
@@ -1293,8 +1412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BO35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
inclusion of existing ship calculations
</commit_message>
<xml_diff>
--- a/data/fuels.xlsx
+++ b/data/fuels.xlsx
@@ -248,16 +248,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>86260</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19585</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>27362</xdr:colOff>
+      <xdr:colOff>141662</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -274,7 +274,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6619875" y="467260"/>
+          <a:off x="6734175" y="591085"/>
           <a:ext cx="4989887" cy="2418815"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1413,7 +1413,7 @@
   <dimension ref="B2:BO35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>